<commit_message>
changes in facilities commit
</commit_message>
<xml_diff>
--- a/sample5.xlsx
+++ b/sample5.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,32 +429,37 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Message</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>company</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>qualififcation</t>
+          <t>event</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>experience</t>
+          <t>linkedin</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>website</t>
         </is>
       </c>
     </row>

</xml_diff>